<commit_message>
OW-535 updated the bilateral trade portfolio to match the acuo-data test branch
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneBilateral.xlsx
+++ b/valuation-app/src/test/resources/excel/OneBilateral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IRS-Bilateral" sheetId="1" state="visible" r:id="rId2"/>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Notionaladj</t>
   </si>
   <si>
-    <t xml:space="preserve">ACUOUK2046</t>
+    <t xml:space="preserve">ACUOSG8745</t>
   </si>
   <si>
     <t xml:space="preserve">928581SHELI3PYW91M</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">a9</t>
   </si>
   <si>
-    <t xml:space="preserve">p9</t>
+    <t xml:space="preserve">p1</t>
   </si>
   <si>
     <t xml:space="preserve">South Africa</t>
@@ -323,54 +323,53 @@
   </sheetPr>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:AR2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
OW-535 renamed some services and review asset valuation service to keep only the latest value per asset
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneBilateral.xlsx
+++ b/valuation-app/src/test/resources/excel/OneBilateral.xlsx
@@ -199,10 +199,10 @@
     <t xml:space="preserve">ZAR-JIBAR-SAFEX</t>
   </si>
   <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
     <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
   </si>
   <si>
     <t xml:space="preserve">5513008I8OABDX7R9S44</t>
@@ -323,53 +323,53 @@
   </sheetPr>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM2" activeCellId="0" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
OW-535 fixed issues related to margin call generation - where the call were not differentiated between client and cpty calls - we were creatin several step nodes at each generation - we were not matching expected and unrecon calls
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneBilateral.xlsx
+++ b/valuation-app/src/test/resources/excel/OneBilateral.xlsx
@@ -211,7 +211,7 @@
     <t xml:space="preserve">a9</t>
   </si>
   <si>
-    <t xml:space="preserve">p1</t>
+    <t xml:space="preserve">p1a</t>
   </si>
   <si>
     <t xml:space="preserve">South Africa</t>
@@ -323,53 +323,53 @@
   </sheetPr>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM2" activeCellId="0" sqref="AM2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM14" activeCellId="0" sqref="AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>